<commit_message>
Attempted to update files in main branch
</commit_message>
<xml_diff>
--- a/russian_words_log.xlsx
+++ b/russian_words_log.xlsx
@@ -6,7 +6,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -16,18 +16,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <b val="1"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
@@ -53,14 +45,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -143,44 +134,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="156082"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -207,32 +198,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -259,24 +232,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -288,162 +243,166 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="phClr"/>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
@@ -453,293 +412,321 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
-    <col width="10.08984375" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="13.81640625" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="12.453125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="12.1796875" bestFit="1" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>First Searched</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Last Searched</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
         <is>
           <t>Word</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Search Counter</t>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Count</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>kris</t>
+          <t>2025-08-05</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>kringle</t>
+          <t>2025-08-06</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>test</t>
-        </is>
+          <t>кошка</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>59</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-07-09</t>
+          <t>2025-08-05</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>да</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>11</v>
+          <t>2025-08-05</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>кош</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-07-16</t>
+          <t>2025-08-05</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>кошка</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>23</v>
+          <t>2025-08-05</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>к</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-07-09</t>
+          <t>2025-08-05</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>кош</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>1</v>
+          <t>2025-08-06</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>ко</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-07-14</t>
+          <t>2025-08-05</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>кот</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>8</v>
+          <t>2025-08-06</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>наряду</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>46</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-07-14</t>
+          <t>2025-08-05</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ток</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>9</v>
+          <t>2025-08-05</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>отряда</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-07-14</t>
+          <t>2025-08-05</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>купить</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>1</v>
+          <t>2025-08-05</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>отряд</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-07-14</t>
+          <t>2025-08-06</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>шифр</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>1</v>
+          <t>2025-08-06</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>ряд</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-07-14</t>
+          <t>2025-08-06</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>расшифровка</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>1</v>
+          <t>2025-08-06</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>капитель</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-07-14</t>
+          <t>2025-08-06</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>привет</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
+          <t>2025-08-06</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>мне</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-07-14</t>
+          <t>2025-08-06</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>добрый день</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
+          <t>2025-08-06</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>до</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-07-14</t>
+          <t>2025-08-06</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>я</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
+          <t>2025-08-06</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>д</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-07-14</t>
+          <t>2025-08-06</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>мой</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
+          <t>2025-08-06</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>буква</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-07-15</t>
+          <t>2025-08-06</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>дверь</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>2025-07-15</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>двор</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>2025-07-15</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>что</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
+          <t>2025-08-06</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>азбука</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>2025-07-15</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>сколько</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>